<commit_message>
Add tests for nested select one, select multiple and gps data
</commit_message>
<xml_diff>
--- a/onadata/apps/main/tests/fixtures/transportation/transportation.xlsx
+++ b/onadata/apps/main/tests/fixtures/transportation/transportation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -88,6 +88,30 @@
     <t xml:space="preserve">Does this hospital have HIV medication?</t>
   </si>
   <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input gps coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple pizza_toppings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza_topping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What toppings to do you prefer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_satisfaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you satisfied with the level of service received?</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin repeat</t>
   </si>
   <si>
@@ -113,6 +137,27 @@
   </si>
   <si>
     <t xml:space="preserve">Last name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">select_multiple </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">pizza_toppings</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">integer</t>
@@ -263,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -305,6 +350,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -388,7 +439,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,16 +502,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.71"/>
@@ -567,85 +618,88 @@
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>23</v>
@@ -653,37 +707,112 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -703,7 +832,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -716,7 +845,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -727,46 +856,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -775,10 +904,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -786,10 +915,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -797,10 +926,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -808,10 +937,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -820,10 +949,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -831,10 +960,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -842,10 +971,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -853,33 +982,33 @@
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -889,46 +1018,46 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -949,7 +1078,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -961,10 +1090,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -972,10 +1101,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>

</xml_diff>